<commit_message>
Doc: CDC + planfication
Planification finie et version 1.0 du CDC
</commit_message>
<xml_diff>
--- a/Doc/TB-Planificattion-ChatillonJeremie.xlsx
+++ b/Doc/TB-Planificattion-ChatillonJeremie.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremie Chatillon\Documents\HEIG\BA-06\TB\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremie Chatillon\Documents\HEIG\BA-06\TB\TB_CleanVotingMap\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93331436-7793-4DEC-B594-E6AF2D56DBCB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D13A2A-9763-47E9-B17D-966C001F4B52}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B3B97FA2-F7FB-4522-96AC-BB53EC21DA80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B3B97FA2-F7FB-4522-96AC-BB53EC21DA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Tâches" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="60">
   <si>
     <t>Taches</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>Analyse</t>
-  </si>
-  <si>
-    <t>Décision sur le comment, quoi,  pourquoi, ou… de toutes les Tâches de type *Concéption*.</t>
   </si>
   <si>
     <t>Architecture</t>
@@ -195,18 +192,6 @@
     <t>Avant les rendus</t>
   </si>
   <si>
-    <t>première phase de con</t>
-  </si>
-  <si>
-    <t>Première phase de concéption</t>
-  </si>
-  <si>
-    <t>Seconde phase de concéption</t>
-  </si>
-  <si>
-    <t>Après le back-end et le front-end</t>
-  </si>
-  <si>
     <t>Totaux</t>
   </si>
   <si>
@@ -222,15 +207,9 @@
     <t>Documentation</t>
   </si>
   <si>
-    <t>. Modélisation de l'application, prise de décision sur l'architecture.  Comprends la phase d'aprentissage + recherches. Modélisation des donnés</t>
-  </si>
-  <si>
     <t>Dev</t>
   </si>
   <si>
-    <t>Choix de l'architecture/ Choix de l'infa</t>
-  </si>
-  <si>
     <t>quoi</t>
   </si>
   <si>
@@ -238,6 +217,38 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Choix de l'architecture / Choix de l'infa</t>
+  </si>
+  <si>
+    <t>Modélisation de l'application, prise de décision sur l'architecture. 
+Modélisation des donnés.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Décision sur le comment, quoi,  pourquoi, ou… de toutes les Tâches de type *Concéption*.
+ Comprends la phase d'aprentissage + recherches. </t>
+  </si>
+  <si>
+    <t>Première phase de conception</t>
+  </si>
+  <si>
+    <t>Seconde  phase de conception</t>
+  </si>
+  <si>
+    <t>troisième  phase de conception</t>
+  </si>
+  <si>
+    <t>Première phase de développement</t>
+  </si>
+  <si>
+    <t>Dernière phase de développement</t>
+  </si>
+  <si>
+    <t>Après le back-end ou le front-end</t>
+  </si>
+  <si>
+    <t>Seconde phase de développement</t>
   </si>
 </sst>
 </file>
@@ -909,12 +920,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -935,16 +940,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -957,98 +956,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1367,8 +1378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C429A887-2864-47AC-8FE3-E0D4CAE19EE3}">
   <dimension ref="B4:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,275 +1397,281 @@
   <sheetData>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="47" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="74" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="53" t="s">
+      <c r="B6" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="53" t="s">
+      <c r="E6" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="48">
         <v>25</v>
       </c>
-      <c r="H6" s="54">
+      <c r="H6" s="65">
         <f>SUM(G6:G8)</f>
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="71"/>
-      <c r="C7" s="53" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="53" t="s">
+      <c r="E7" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="48">
+        <v>100</v>
+      </c>
+      <c r="H7" s="66"/>
+    </row>
+    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="70"/>
+      <c r="C8" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="53">
-        <v>100</v>
-      </c>
-      <c r="H7" s="56"/>
-    </row>
-    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="73"/>
-      <c r="C8" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="65" t="s">
+      <c r="G8" s="56">
+        <v>10</v>
+      </c>
+      <c r="H8" s="67"/>
+    </row>
+    <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="68" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="48">
         <v>30</v>
       </c>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="65">
-        <v>10</v>
-      </c>
-      <c r="H8" s="64"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="72" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="53">
-        <v>30</v>
-      </c>
-      <c r="H9" s="67">
+      <c r="H9" s="64">
         <f>SUM(G9:G11)</f>
         <v>80</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="69"/>
+      <c r="C10" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="71"/>
-      <c r="C10" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53">
+      <c r="G10" s="48">
         <v>30</v>
       </c>
-      <c r="H10" s="57"/>
+      <c r="H10" s="62"/>
       <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="70"/>
+      <c r="C11" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="73"/>
-      <c r="C11" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="53">
+      <c r="G11" s="48">
         <v>20</v>
       </c>
-      <c r="H11" s="68"/>
+      <c r="H11" s="63"/>
       <c r="J11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="68" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="53" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="66">
+      <c r="G12" s="57">
         <v>40</v>
       </c>
-      <c r="H12" s="57">
+      <c r="H12" s="62">
         <f>SUM(G12:G15)</f>
         <v>150</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="71"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="69"/>
+      <c r="C13" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53">
+      <c r="E13" s="48"/>
+      <c r="F13" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="48">
         <v>40</v>
       </c>
-      <c r="H13" s="57"/>
+      <c r="H13" s="62"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="71"/>
-      <c r="C14" s="53" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53" t="s">
+      <c r="E14" s="48"/>
+      <c r="F14" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="48">
+        <v>30</v>
+      </c>
+      <c r="H14" s="62"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="70"/>
+      <c r="C15" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="56">
+        <v>40</v>
+      </c>
+      <c r="H15" s="63"/>
+    </row>
+    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="58">
         <v>45</v>
       </c>
-      <c r="G14" s="53">
-        <v>30</v>
-      </c>
-      <c r="H14" s="57"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="73"/>
-      <c r="C15" s="65" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="65">
+      <c r="H16" s="59">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="50">
         <v>40</v>
       </c>
-      <c r="H15" s="68"/>
-    </row>
-    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="69">
-        <v>45</v>
-      </c>
-      <c r="H16" s="70">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="58" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="58">
+      <c r="H17" s="51">
         <v>40</v>
       </c>
-      <c r="H17" s="59">
-        <v>40</v>
-      </c>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="62">
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="54">
         <f ca="1">SUM(G6:G27)</f>
         <v>450</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="55">
         <f>SUM(H6:H17)</f>
         <v>450</v>
       </c>
@@ -1676,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8458467-B4D6-4FF3-B258-BB5B16F11DDF}">
   <dimension ref="A1:BJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29:X29"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="AT8" sqref="AT8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,11 +1754,11 @@
       <c r="AW1" s="5"/>
     </row>
     <row r="2" spans="1:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>28</v>
+      <c r="B2" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>27</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1758,7 +1775,7 @@
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="I2" s="40">
+      <c r="I2" s="36">
         <v>6</v>
       </c>
       <c r="J2">
@@ -1791,53 +1808,53 @@
       <c r="S2">
         <v>16</v>
       </c>
-      <c r="T2" s="39">
+      <c r="T2" s="76">
         <v>17</v>
       </c>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="18">
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="73">
         <v>18</v>
       </c>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="18">
+      <c r="Z2" s="73"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="74"/>
+      <c r="AD2" s="73">
         <v>19</v>
       </c>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="34"/>
-      <c r="AI2" s="18">
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="73">
         <v>20</v>
       </c>
-      <c r="AJ2" s="18"/>
-      <c r="AK2" s="18"/>
-      <c r="AL2" s="18"/>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="18">
+      <c r="AJ2" s="73"/>
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="73"/>
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="73">
         <v>21</v>
       </c>
-      <c r="AO2" s="18"/>
-      <c r="AP2" s="18"/>
-      <c r="AQ2" s="18"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="18">
+      <c r="AO2" s="73"/>
+      <c r="AP2" s="73"/>
+      <c r="AQ2" s="73"/>
+      <c r="AR2" s="74"/>
+      <c r="AS2" s="73">
         <v>22</v>
       </c>
-      <c r="AT2" s="18"/>
-      <c r="AU2" s="18"/>
-      <c r="AV2" s="18"/>
-      <c r="AW2" s="19"/>
+      <c r="AT2" s="73"/>
+      <c r="AU2" s="73"/>
+      <c r="AV2" s="73"/>
+      <c r="AW2" s="75"/>
     </row>
     <row r="3" spans="1:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="46"/>
-      <c r="C3" s="45" t="s">
-        <v>39</v>
+      <c r="B3" s="72"/>
+      <c r="C3" s="41" t="s">
+        <v>38</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -1856,106 +1873,106 @@
       <c r="R3" s="5"/>
       <c r="S3" s="6"/>
       <c r="T3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="5" t="s">
+      <c r="V3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="5" t="s">
+      <c r="X3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="W3" s="5" t="s">
+      <c r="AC3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y3" s="5" t="s">
+      <c r="AD3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="AF3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="AH3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="5" t="s">
+      <c r="AM3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="AC3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD3" s="5" t="s">
+      <c r="AN3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AP3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AF3" s="5" t="s">
+      <c r="AR3" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="AS3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AG3" s="5" t="s">
+      <c r="AW3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AH3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AQ3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AR3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="AS3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AU3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AV3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AW3" s="16" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="4" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="25">
+      <c r="A4" s="37"/>
+      <c r="B4" s="23">
         <f>SUM(D4:AW4)</f>
         <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <v>12</v>
       </c>
       <c r="E4" s="3">
@@ -1965,20 +1982,20 @@
         <v>1</v>
       </c>
       <c r="S4" s="2"/>
-      <c r="X4" s="29"/>
-      <c r="AC4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AR4" s="30"/>
+      <c r="X4" s="27"/>
+      <c r="AC4" s="28"/>
+      <c r="AH4" s="28"/>
+      <c r="AM4" s="28"/>
+      <c r="AR4" s="28"/>
       <c r="AW4" s="14"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
-      <c r="B5" s="47">
+      <c r="B5" s="42">
         <f t="shared" ref="B5:B27" si="0">SUM(D5:AW5)</f>
         <v>15</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="19">
         <v>12</v>
       </c>
       <c r="E5" s="4">
@@ -1986,23 +2003,23 @@
       </c>
       <c r="F5" s="4"/>
       <c r="S5" s="2"/>
-      <c r="X5" s="30"/>
-      <c r="AC5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AM5" s="30"/>
-      <c r="AR5" s="30"/>
+      <c r="X5" s="28"/>
+      <c r="AC5" s="28"/>
+      <c r="AH5" s="28"/>
+      <c r="AM5" s="28"/>
+      <c r="AR5" s="28"/>
       <c r="AW5" s="14"/>
     </row>
     <row r="6" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="48">
+      <c r="A6" s="37"/>
+      <c r="B6" s="43">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="20"/>
       <c r="G6" s="9">
         <v>4</v>
       </c>
@@ -2039,16 +2056,16 @@
       <c r="R6" s="9">
         <v>2</v>
       </c>
-      <c r="S6" s="28"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="33"/>
+      <c r="U6" s="33"/>
       <c r="V6" s="9">
         <v>2</v>
       </c>
       <c r="W6" s="9">
         <v>2</v>
       </c>
-      <c r="X6" s="31">
+      <c r="X6" s="29">
         <v>2</v>
       </c>
       <c r="Y6" s="9">
@@ -2063,8 +2080,8 @@
       <c r="AB6" s="9">
         <v>2</v>
       </c>
-      <c r="AC6" s="38"/>
-      <c r="AD6" s="36"/>
+      <c r="AC6" s="35"/>
+      <c r="AD6" s="33"/>
       <c r="AE6" s="9">
         <v>2</v>
       </c>
@@ -2074,7 +2091,7 @@
       <c r="AG6" s="9">
         <v>2</v>
       </c>
-      <c r="AH6" s="31">
+      <c r="AH6" s="29">
         <v>3</v>
       </c>
       <c r="AI6" s="9">
@@ -2083,9 +2100,9 @@
       <c r="AJ6" s="9">
         <v>2</v>
       </c>
-      <c r="AK6" s="36"/>
-      <c r="AL6" s="36"/>
-      <c r="AM6" s="38"/>
+      <c r="AK6" s="33"/>
+      <c r="AL6" s="33"/>
+      <c r="AM6" s="35"/>
       <c r="AN6" s="9">
         <v>2</v>
       </c>
@@ -2098,7 +2115,7 @@
       <c r="AQ6" s="9">
         <v>3</v>
       </c>
-      <c r="AR6" s="31">
+      <c r="AR6" s="29">
         <v>3</v>
       </c>
       <c r="AS6" s="9">
@@ -2111,7 +2128,7 @@
         <v>9</v>
       </c>
       <c r="AV6" s="9"/>
-      <c r="AW6" s="37"/>
+      <c r="AW6" s="34"/>
       <c r="AX6" s="12"/>
       <c r="AY6" s="12"/>
       <c r="AZ6" s="12"/>
@@ -2128,30 +2145,30 @@
     </row>
     <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="49">
+      <c r="B7" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="23"/>
+      <c r="D7" s="21"/>
       <c r="S7" s="2"/>
-      <c r="X7" s="30"/>
-      <c r="AC7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AM7" s="30"/>
-      <c r="AR7" s="30"/>
+      <c r="X7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AR7" s="28"/>
       <c r="AW7" s="14"/>
     </row>
     <row r="8" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="26">
+      <c r="A8" s="37"/>
+      <c r="B8" s="24">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="20"/>
       <c r="F8" s="9">
         <v>9</v>
       </c>
@@ -2165,11 +2182,11 @@
         <v>5</v>
       </c>
       <c r="S8" s="11"/>
-      <c r="X8" s="32"/>
-      <c r="AC8" s="32"/>
-      <c r="AH8" s="32"/>
-      <c r="AM8" s="32"/>
-      <c r="AR8" s="32"/>
+      <c r="X8" s="30"/>
+      <c r="AC8" s="30"/>
+      <c r="AH8" s="30"/>
+      <c r="AM8" s="30"/>
+      <c r="AR8" s="30"/>
       <c r="AW8" s="17"/>
       <c r="AX8" s="12"/>
       <c r="AY8" s="12"/>
@@ -2187,30 +2204,30 @@
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="47">
+      <c r="B9" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="21"/>
       <c r="S9" s="2"/>
-      <c r="X9" s="30"/>
-      <c r="AC9" s="30"/>
-      <c r="AH9" s="30"/>
-      <c r="AM9" s="30"/>
-      <c r="AR9" s="30"/>
+      <c r="X9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AM9" s="28"/>
+      <c r="AR9" s="28"/>
       <c r="AW9" s="14"/>
     </row>
     <row r="10" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="48">
+      <c r="A10" s="37"/>
+      <c r="B10" s="43">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="20"/>
       <c r="I10" s="9">
         <v>3</v>
       </c>
@@ -2224,11 +2241,11 @@
         <v>9</v>
       </c>
       <c r="S10" s="11"/>
-      <c r="X10" s="32"/>
-      <c r="AC10" s="32"/>
-      <c r="AH10" s="32"/>
-      <c r="AM10" s="32"/>
-      <c r="AR10" s="32"/>
+      <c r="X10" s="30"/>
+      <c r="AC10" s="30"/>
+      <c r="AH10" s="30"/>
+      <c r="AM10" s="30"/>
+      <c r="AR10" s="30"/>
       <c r="AW10" s="17"/>
       <c r="AX10" s="12"/>
       <c r="AY10" s="12"/>
@@ -2246,30 +2263,30 @@
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="49">
+      <c r="B11" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="21"/>
       <c r="S11" s="2"/>
-      <c r="X11" s="30"/>
-      <c r="AC11" s="30"/>
-      <c r="AH11" s="30"/>
-      <c r="AM11" s="30"/>
-      <c r="AR11" s="30"/>
+      <c r="X11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AH11" s="28"/>
+      <c r="AM11" s="28"/>
+      <c r="AR11" s="28"/>
       <c r="AW11" s="14"/>
     </row>
     <row r="12" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="26">
+      <c r="A12" s="37"/>
+      <c r="B12" s="24">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="22"/>
+        <v>26</v>
+      </c>
+      <c r="D12" s="20"/>
       <c r="M12" s="9">
         <v>10</v>
       </c>
@@ -2277,11 +2294,11 @@
         <v>10</v>
       </c>
       <c r="S12" s="11"/>
-      <c r="X12" s="32"/>
-      <c r="AC12" s="32"/>
-      <c r="AH12" s="32"/>
-      <c r="AM12" s="32"/>
-      <c r="AR12" s="32"/>
+      <c r="X12" s="30"/>
+      <c r="AC12" s="30"/>
+      <c r="AH12" s="30"/>
+      <c r="AM12" s="30"/>
+      <c r="AR12" s="30"/>
       <c r="AW12" s="17"/>
       <c r="AX12" s="12"/>
       <c r="AY12" s="12"/>
@@ -2299,30 +2316,30 @@
     </row>
     <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="49">
+      <c r="B13" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="21"/>
       <c r="S13" s="2"/>
-      <c r="X13" s="30"/>
-      <c r="AC13" s="30"/>
-      <c r="AH13" s="30"/>
-      <c r="AM13" s="30"/>
-      <c r="AR13" s="30"/>
+      <c r="X13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AR13" s="28"/>
       <c r="AW13" s="14"/>
     </row>
     <row r="14" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="48">
+      <c r="A14" s="37"/>
+      <c r="B14" s="43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="20"/>
       <c r="O14" s="9">
         <v>10</v>
       </c>
@@ -2336,11 +2353,11 @@
         <v>10</v>
       </c>
       <c r="S14" s="11"/>
-      <c r="X14" s="32"/>
-      <c r="AC14" s="32"/>
-      <c r="AH14" s="32"/>
-      <c r="AM14" s="32"/>
-      <c r="AR14" s="32"/>
+      <c r="X14" s="30"/>
+      <c r="AC14" s="30"/>
+      <c r="AH14" s="30"/>
+      <c r="AM14" s="30"/>
+      <c r="AR14" s="30"/>
       <c r="AW14" s="17"/>
       <c r="AX14" s="12"/>
       <c r="AY14" s="12"/>
@@ -2358,33 +2375,33 @@
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="49">
+      <c r="B15" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="21"/>
       <c r="S15" s="2"/>
-      <c r="X15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AH15" s="30"/>
-      <c r="AM15" s="30"/>
-      <c r="AR15" s="30"/>
+      <c r="X15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AH15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AR15" s="28"/>
       <c r="AW15" s="14"/>
     </row>
     <row r="16" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="26">
+      <c r="A16" s="37"/>
+      <c r="B16" s="24">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="20"/>
       <c r="S16" s="11"/>
-      <c r="X16" s="32"/>
-      <c r="AC16" s="31">
+      <c r="X16" s="30"/>
+      <c r="AC16" s="29">
         <v>8</v>
       </c>
       <c r="AD16" s="9">
@@ -2402,8 +2419,8 @@
       <c r="AH16" s="9">
         <v>3</v>
       </c>
-      <c r="AM16" s="32"/>
-      <c r="AR16" s="32"/>
+      <c r="AM16" s="30"/>
+      <c r="AR16" s="30"/>
       <c r="AW16" s="17"/>
       <c r="AX16" s="12"/>
       <c r="AY16" s="12"/>
@@ -2421,32 +2438,32 @@
     </row>
     <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="47">
+      <c r="B17" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="21"/>
       <c r="S17" s="2"/>
-      <c r="X17" s="30"/>
-      <c r="AC17" s="30"/>
-      <c r="AH17" s="30"/>
-      <c r="AM17" s="30"/>
-      <c r="AR17" s="30"/>
+      <c r="X17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AH17" s="28"/>
+      <c r="AM17" s="28"/>
+      <c r="AR17" s="28"/>
       <c r="AW17" s="14"/>
     </row>
     <row r="18" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="48">
+      <c r="A18" s="37"/>
+      <c r="B18" s="43">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="20"/>
       <c r="S18" s="11"/>
-      <c r="X18" s="32"/>
+      <c r="X18" s="30"/>
       <c r="Z18" s="9">
         <v>7</v>
       </c>
@@ -2456,16 +2473,16 @@
       <c r="AB18" s="9">
         <v>5</v>
       </c>
-      <c r="AC18" s="32"/>
-      <c r="AH18" s="32"/>
+      <c r="AC18" s="30"/>
+      <c r="AH18" s="30"/>
       <c r="AI18" s="9">
         <v>6</v>
       </c>
       <c r="AJ18" s="9">
         <v>5</v>
       </c>
-      <c r="AM18" s="32"/>
-      <c r="AR18" s="32"/>
+      <c r="AM18" s="30"/>
+      <c r="AR18" s="30"/>
       <c r="AW18" s="17"/>
       <c r="AX18" s="12"/>
       <c r="AY18" s="12"/>
@@ -2483,30 +2500,30 @@
     </row>
     <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
-      <c r="B19" s="47">
+      <c r="B19" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="23"/>
+      <c r="D19" s="21"/>
       <c r="S19" s="2"/>
-      <c r="X19" s="30"/>
-      <c r="AC19" s="30"/>
-      <c r="AH19" s="30"/>
-      <c r="AM19" s="30"/>
-      <c r="AR19" s="30"/>
+      <c r="X19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AM19" s="28"/>
+      <c r="AR19" s="28"/>
       <c r="AW19" s="14"/>
     </row>
     <row r="20" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41"/>
-      <c r="B20" s="48">
+      <c r="A20" s="37"/>
+      <c r="B20" s="43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="20"/>
       <c r="S20" s="11"/>
       <c r="T20" s="9">
         <v>8</v>
@@ -2526,10 +2543,10 @@
       <c r="Y20" s="9">
         <v>3</v>
       </c>
-      <c r="AC20" s="32"/>
-      <c r="AH20" s="32"/>
-      <c r="AM20" s="32"/>
-      <c r="AR20" s="32"/>
+      <c r="AC20" s="30"/>
+      <c r="AH20" s="30"/>
+      <c r="AM20" s="30"/>
+      <c r="AR20" s="30"/>
       <c r="AW20" s="17"/>
       <c r="AX20" s="12"/>
       <c r="AY20" s="12"/>
@@ -2547,38 +2564,38 @@
     </row>
     <row r="21" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
-      <c r="B21" s="49">
+      <c r="B21" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="23"/>
+      <c r="D21" s="21"/>
       <c r="S21" s="2"/>
-      <c r="X21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AH21" s="30"/>
-      <c r="AM21" s="30"/>
-      <c r="AR21" s="30"/>
+      <c r="X21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AH21" s="28"/>
+      <c r="AM21" s="28"/>
+      <c r="AR21" s="28"/>
       <c r="AW21" s="14"/>
     </row>
     <row r="22" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="47">
+      <c r="A22" s="37"/>
+      <c r="B22" s="42">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="20"/>
       <c r="S22" s="11"/>
-      <c r="X22" s="32"/>
-      <c r="AC22" s="32"/>
-      <c r="AH22" s="32"/>
+      <c r="X22" s="30"/>
+      <c r="AC22" s="30"/>
+      <c r="AH22" s="30"/>
       <c r="AL22" s="9">
         <v>9</v>
       </c>
-      <c r="AM22" s="31">
+      <c r="AM22" s="29">
         <v>8</v>
       </c>
       <c r="AN22" s="9">
@@ -2593,7 +2610,7 @@
       <c r="AQ22" s="9">
         <v>6</v>
       </c>
-      <c r="AR22" s="31">
+      <c r="AR22" s="29">
         <v>3</v>
       </c>
       <c r="AW22" s="17"/>
@@ -2613,38 +2630,38 @@
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
-      <c r="B23" s="26">
+      <c r="B23" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="23"/>
+      <c r="D23" s="21"/>
       <c r="S23" s="2"/>
-      <c r="X23" s="30"/>
-      <c r="AC23" s="30"/>
-      <c r="AH23" s="30"/>
-      <c r="AM23" s="30"/>
-      <c r="AR23" s="30"/>
+      <c r="X23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AH23" s="28"/>
+      <c r="AM23" s="28"/>
+      <c r="AR23" s="28"/>
       <c r="AW23" s="14"/>
     </row>
     <row r="24" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41"/>
-      <c r="B24" s="48">
+      <c r="A24" s="37"/>
+      <c r="B24" s="43">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="22"/>
+        <v>28</v>
+      </c>
+      <c r="D24" s="20"/>
       <c r="S24" s="10">
         <v>5</v>
       </c>
-      <c r="X24" s="32"/>
-      <c r="AC24" s="32"/>
-      <c r="AH24" s="32"/>
-      <c r="AM24" s="32"/>
-      <c r="AR24" s="32"/>
+      <c r="X24" s="30"/>
+      <c r="AC24" s="30"/>
+      <c r="AH24" s="30"/>
+      <c r="AM24" s="30"/>
+      <c r="AR24" s="30"/>
       <c r="AV24" s="9">
         <v>5</v>
       </c>
@@ -2665,45 +2682,45 @@
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="B25" s="47">
+      <c r="B25" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="23"/>
+      <c r="D25" s="21"/>
       <c r="S25" s="2"/>
-      <c r="X25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AH25" s="30"/>
-      <c r="AM25" s="30"/>
-      <c r="AR25" s="30"/>
+      <c r="X25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AH25" s="28"/>
+      <c r="AM25" s="28"/>
+      <c r="AR25" s="28"/>
       <c r="AW25" s="14"/>
     </row>
     <row r="26" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="41"/>
-      <c r="B26" s="48">
+      <c r="A26" s="37"/>
+      <c r="B26" s="43">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="22"/>
+      <c r="D26" s="20"/>
       <c r="F26" s="9">
         <v>2</v>
       </c>
       <c r="S26" s="10">
         <v>7</v>
       </c>
-      <c r="X26" s="32"/>
+      <c r="X26" s="30"/>
       <c r="Y26" s="9">
         <v>2</v>
       </c>
       <c r="AB26" s="9">
         <v>2</v>
       </c>
-      <c r="AC26" s="32"/>
-      <c r="AH26" s="31">
+      <c r="AC26" s="30"/>
+      <c r="AH26" s="29">
         <v>2</v>
       </c>
       <c r="AJ26" s="9">
@@ -2712,14 +2729,14 @@
       <c r="AK26" s="9">
         <v>9</v>
       </c>
-      <c r="AM26" s="32"/>
-      <c r="AR26" s="31">
+      <c r="AM26" s="30"/>
+      <c r="AR26" s="29">
         <v>2</v>
       </c>
       <c r="AV26" s="9">
         <v>4</v>
       </c>
-      <c r="AW26" s="35">
+      <c r="AW26" s="32">
         <v>8</v>
       </c>
       <c r="AX26" s="12"/>
@@ -2738,12 +2755,12 @@
     </row>
     <row r="27" spans="1:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
-      <c r="B27" s="27">
+      <c r="B27" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C27" s="16"/>
-      <c r="D27" s="24"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2763,27 +2780,27 @@
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
-      <c r="X27" s="33"/>
+      <c r="X27" s="31"/>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
-      <c r="AC27" s="33"/>
+      <c r="AC27" s="31"/>
       <c r="AD27" s="5"/>
       <c r="AE27" s="5"/>
       <c r="AF27" s="5"/>
       <c r="AG27" s="5"/>
-      <c r="AH27" s="33"/>
+      <c r="AH27" s="31"/>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
       <c r="AK27" s="5"/>
       <c r="AL27" s="5"/>
-      <c r="AM27" s="33"/>
+      <c r="AM27" s="31"/>
       <c r="AN27" s="5"/>
       <c r="AO27" s="5"/>
       <c r="AP27" s="5"/>
       <c r="AQ27" s="5"/>
-      <c r="AR27" s="33"/>
+      <c r="AR27" s="31"/>
       <c r="AS27" s="5"/>
       <c r="AT27" s="5"/>
       <c r="AU27" s="5"/>
@@ -2792,195 +2809,195 @@
     </row>
     <row r="28" spans="1:62" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="42">
+      <c r="B28" s="38">
         <f>SUM(B4,B6,B8,B10,B12,B14,B16,B18,B20,B22,B24,B26)</f>
         <v>450</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28">
-        <f>SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20,D22,D24,D26)</f>
+        <f t="shared" ref="D28:S28" si="1">SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20,D22,D24,D26)</f>
         <v>12</v>
       </c>
       <c r="E28">
-        <f>SUM(E4,E6,E8,E10,E12,E14,E16,E18,E20,E22,E24,E26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="F28">
-        <f>SUM(F4,F6,F8,F10,F12,F14,F16,F18,F20,F22,F24,F26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="G28">
-        <f>SUM(G4,G6,G8,G10,G12,G14,G16,G18,G20,G22,G24,G26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H28">
-        <f>SUM(H4,H6,H8,H10,H12,H14,H16,H18,H20,H22,H24,H26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I28">
-        <f>SUM(I4,I6,I8,I10,I12,I14,I16,I18,I20,I22,I24,I26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="J28">
-        <f>SUM(J4,J6,J8,J10,J12,J14,J16,J18,J20,J22,J24,J26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="K28">
-        <f>SUM(K4,K6,K8,K10,K12,K14,K16,K18,K20,K22,K24,K26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="L28">
-        <f>SUM(L4,L6,L8,L10,L12,L14,L16,L18,L20,L22,L24,L26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="M28">
-        <f>SUM(M4,M6,M8,M10,M12,M14,M16,M18,M20,M22,M24,M26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="N28">
-        <f>SUM(N4,N6,N8,N10,N12,N14,N16,N18,N20,N22,N24,N26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="O28">
-        <f>SUM(O4,O6,O8,O10,O12,O14,O16,O18,O20,O22,O24,O26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="P28">
-        <f>SUM(P4,P6,P8,P10,P12,P14,P16,P18,P20,P22,P24,P26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="Q28">
-        <f>SUM(Q4,Q6,Q8,Q10,Q12,Q14,Q16,Q18,Q20,Q22,Q24,Q26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="R28">
-        <f>SUM(R4,R6,R8,R10,R12,R14,R16,R18,R20,R22,R24,R26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="S28" s="13">
-        <f>SUM(S4,S6,S8,S10,S12,S14,S16,S18,S20,S22,S24,S26)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="T28">
-        <f t="shared" ref="T28:AW28" si="1">SUM(T4,T6,T8,T10,T12,T14,T16,T18,T20,T22,T24,T26)</f>
+        <f t="shared" ref="T28:AW28" si="2">SUM(T4,T6,T8,T10,T12,T14,T16,T18,T20,T22,T24,T26)</f>
         <v>8</v>
       </c>
       <c r="U28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="V28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="W28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="X28" s="30">
-        <f t="shared" si="1"/>
+      <c r="X28" s="28">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AH28" s="30">
-        <f t="shared" si="1"/>
+      <c r="AH28" s="28">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AI28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AJ28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AK28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AL28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AM28" s="30">
-        <f t="shared" si="1"/>
+      <c r="AM28" s="28">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AQ28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="AR28" s="30">
-        <f t="shared" si="1"/>
+      <c r="AR28" s="28">
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AS28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AT28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AU28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AV28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AW28" s="15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="AX28" s="12"/>
@@ -3003,7 +3020,7 @@
         <f>SUM(B5,B7,B9,B11,B13,B15,B17,B19,B21,B23,B25,B27)</f>
         <v>15</v>
       </c>
-      <c r="C29" s="43">
+      <c r="C29" s="39">
         <f>SUM(D28:AW28)</f>
         <v>450</v>
       </c>
@@ -3012,145 +3029,145 @@
         <v>12</v>
       </c>
       <c r="E29">
-        <f t="shared" ref="E29:S29" si="2">SUM(E5,E7,E9,E11,E13,E15,E17,E19,E21,E23,E25,E27)</f>
+        <f t="shared" ref="E29:S29" si="3">SUM(E5,E7,E9,E11,E13,E15,E17,E19,E21,E23,E25,E27)</f>
         <v>3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="T29" s="18"/>
-      <c r="U29" s="18"/>
-      <c r="V29" s="18"/>
-      <c r="W29" s="18"/>
-      <c r="X29" s="34"/>
-      <c r="Y29" s="18"/>
-      <c r="Z29" s="18"/>
-      <c r="AA29" s="18"/>
-      <c r="AB29" s="18"/>
-      <c r="AC29" s="34"/>
-      <c r="AD29" s="18"/>
-      <c r="AE29" s="18"/>
-      <c r="AF29" s="18"/>
-      <c r="AG29" s="18"/>
-      <c r="AH29" s="34"/>
-      <c r="AI29" s="18"/>
-      <c r="AJ29" s="18"/>
-      <c r="AK29" s="18"/>
-      <c r="AL29" s="18"/>
-      <c r="AM29" s="34"/>
-      <c r="AN29" s="18"/>
-      <c r="AO29" s="18"/>
-      <c r="AP29" s="18"/>
-      <c r="AQ29" s="18"/>
-      <c r="AR29" s="34"/>
-      <c r="AS29" s="18"/>
-      <c r="AT29" s="18"/>
-      <c r="AU29" s="18"/>
-      <c r="AV29" s="18"/>
-      <c r="AW29" s="19"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="73"/>
+      <c r="V29" s="73"/>
+      <c r="W29" s="73"/>
+      <c r="X29" s="74"/>
+      <c r="Y29" s="73"/>
+      <c r="Z29" s="73"/>
+      <c r="AA29" s="73"/>
+      <c r="AB29" s="73"/>
+      <c r="AC29" s="74"/>
+      <c r="AD29" s="73"/>
+      <c r="AE29" s="73"/>
+      <c r="AF29" s="73"/>
+      <c r="AG29" s="73"/>
+      <c r="AH29" s="74"/>
+      <c r="AI29" s="73"/>
+      <c r="AJ29" s="73"/>
+      <c r="AK29" s="73"/>
+      <c r="AL29" s="73"/>
+      <c r="AM29" s="74"/>
+      <c r="AN29" s="73"/>
+      <c r="AO29" s="73"/>
+      <c r="AP29" s="73"/>
+      <c r="AQ29" s="73"/>
+      <c r="AR29" s="74"/>
+      <c r="AS29" s="73"/>
+      <c r="AT29" s="73"/>
+      <c r="AU29" s="73"/>
+      <c r="AV29" s="73"/>
+      <c r="AW29" s="75"/>
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
-      <c r="B30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="40"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
-      <c r="P30" s="40"/>
-      <c r="Q30" s="40"/>
-      <c r="R30" s="40"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="40"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="40"/>
-      <c r="X30" s="40"/>
-      <c r="Y30" s="40"/>
-      <c r="Z30" s="40"/>
-      <c r="AA30" s="40"/>
-      <c r="AB30" s="40"/>
-      <c r="AC30" s="40"/>
-      <c r="AD30" s="40"/>
-      <c r="AE30" s="40"/>
-      <c r="AF30" s="40"/>
-      <c r="AG30" s="40"/>
-      <c r="AH30" s="40"/>
-      <c r="AI30" s="40"/>
-      <c r="AJ30" s="40"/>
-      <c r="AK30" s="40"/>
-      <c r="AL30" s="40"/>
-      <c r="AM30" s="40"/>
-      <c r="AN30" s="40"/>
-      <c r="AO30" s="40"/>
-      <c r="AP30" s="40"/>
-      <c r="AQ30" s="40"/>
-      <c r="AR30" s="40"/>
-      <c r="AS30" s="40"/>
-      <c r="AT30" s="40"/>
-      <c r="AU30" s="40"/>
-      <c r="AV30" s="40"/>
-      <c r="AW30" s="40"/>
+      <c r="B30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="36"/>
+      <c r="P30" s="36"/>
+      <c r="Q30" s="36"/>
+      <c r="R30" s="36"/>
+      <c r="S30" s="36"/>
+      <c r="T30" s="36"/>
+      <c r="U30" s="36"/>
+      <c r="V30" s="36"/>
+      <c r="W30" s="36"/>
+      <c r="X30" s="36"/>
+      <c r="Y30" s="36"/>
+      <c r="Z30" s="36"/>
+      <c r="AA30" s="36"/>
+      <c r="AB30" s="36"/>
+      <c r="AC30" s="36"/>
+      <c r="AD30" s="36"/>
+      <c r="AE30" s="36"/>
+      <c r="AF30" s="36"/>
+      <c r="AG30" s="36"/>
+      <c r="AH30" s="36"/>
+      <c r="AI30" s="36"/>
+      <c r="AJ30" s="36"/>
+      <c r="AK30" s="36"/>
+      <c r="AL30" s="36"/>
+      <c r="AM30" s="36"/>
+      <c r="AN30" s="36"/>
+      <c r="AO30" s="36"/>
+      <c r="AP30" s="36"/>
+      <c r="AQ30" s="36"/>
+      <c r="AR30" s="36"/>
+      <c r="AS30" s="36"/>
+      <c r="AT30" s="36"/>
+      <c r="AU30" s="36"/>
+      <c r="AV30" s="36"/>
+      <c r="AW30" s="36"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
@@ -3163,11 +3180,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Y29:AC29"/>
-    <mergeCell ref="AD29:AH29"/>
-    <mergeCell ref="AI29:AM29"/>
     <mergeCell ref="AN29:AR29"/>
     <mergeCell ref="AS29:AW29"/>
     <mergeCell ref="T2:X2"/>
@@ -3176,6 +3188,11 @@
     <mergeCell ref="AI2:AM2"/>
     <mergeCell ref="AN2:AR2"/>
     <mergeCell ref="AS2:AW2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Y29:AC29"/>
+    <mergeCell ref="AD29:AH29"/>
+    <mergeCell ref="AI29:AM29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>